<commit_message>
Se agrego el filtro DBYF
</commit_message>
<xml_diff>
--- a/Catalogo_Normalizado.xlsx
+++ b/Catalogo_Normalizado.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11025" tabRatio="984" activeTab="9"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="11025" tabRatio="984" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Portada" sheetId="187" r:id="rId1"/>
@@ -29,12 +29,12 @@
     <definedName name="PROFUNDIDADES">#REF!</definedName>
     <definedName name="RECREACIÓN">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9089" uniqueCount="3607">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9388" uniqueCount="3608">
   <si>
     <t>01</t>
   </si>
@@ -10873,6 +10873,9 @@
   </si>
   <si>
     <t>Zona 5</t>
+  </si>
+  <si>
+    <t>DBYF</t>
   </si>
 </sst>
 </file>
@@ -11902,7 +11905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E998"/>
     </sheetView>
   </sheetViews>
@@ -28025,10 +28028,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E299"/>
+  <dimension ref="A1:F299"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -28037,10 +28040,10 @@
     <col min="2" max="2" width="9" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="255.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>1995</v>
       </c>
@@ -28056,8 +28059,11 @@
       <c r="E1" t="s">
         <v>1987</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>3607</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>216</v>
       </c>
@@ -28073,8 +28079,11 @@
       <c r="E2" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>216</v>
       </c>
@@ -28090,8 +28099,11 @@
       <c r="E3" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>216</v>
       </c>
@@ -28107,8 +28119,11 @@
       <c r="E4" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -28124,8 +28139,11 @@
       <c r="E5" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>216</v>
       </c>
@@ -28141,8 +28159,11 @@
       <c r="E6" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>216</v>
       </c>
@@ -28158,8 +28179,11 @@
       <c r="E7" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -28175,15 +28199,18 @@
       <c r="E8" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>217</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D9" t="s">
@@ -28192,8 +28219,11 @@
       <c r="E9" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>217</v>
       </c>
@@ -28209,8 +28239,11 @@
       <c r="E10" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>217</v>
       </c>
@@ -28226,8 +28259,11 @@
       <c r="E11" t="s">
         <v>1002</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>217</v>
       </c>
@@ -28243,8 +28279,11 @@
       <c r="E12" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -28260,8 +28299,11 @@
       <c r="E13" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>217</v>
       </c>
@@ -28277,8 +28319,11 @@
       <c r="E14" t="s">
         <v>987</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>217</v>
       </c>
@@ -28294,8 +28339,11 @@
       <c r="E15" t="s">
         <v>1698</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>218</v>
       </c>
@@ -28311,8 +28359,11 @@
       <c r="E16" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>218</v>
       </c>
@@ -28328,8 +28379,11 @@
       <c r="E17" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>218</v>
       </c>
@@ -28345,8 +28399,11 @@
       <c r="E18" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>218</v>
       </c>
@@ -28362,8 +28419,11 @@
       <c r="E19" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>218</v>
       </c>
@@ -28379,8 +28439,11 @@
       <c r="E20" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>218</v>
       </c>
@@ -28396,8 +28459,11 @@
       <c r="E21" t="s">
         <v>1130</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>218</v>
       </c>
@@ -28413,8 +28479,11 @@
       <c r="E22" t="s">
         <v>1846</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>219</v>
       </c>
@@ -28430,8 +28499,11 @@
       <c r="E23" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>219</v>
       </c>
@@ -28447,8 +28519,11 @@
       <c r="E24" t="s">
         <v>1005</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>219</v>
       </c>
@@ -28464,8 +28539,11 @@
       <c r="E25" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>220</v>
       </c>
@@ -28481,8 +28559,11 @@
       <c r="E26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>220</v>
       </c>
@@ -28498,8 +28579,11 @@
       <c r="E27" t="s">
         <v>1682</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>220</v>
       </c>
@@ -28515,8 +28599,11 @@
       <c r="E28" t="s">
         <v>1638</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>220</v>
       </c>
@@ -28532,8 +28619,11 @@
       <c r="E29" t="s">
         <v>1639</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>221</v>
       </c>
@@ -28549,8 +28639,11 @@
       <c r="E30" t="s">
         <v>1699</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>221</v>
       </c>
@@ -28566,8 +28659,11 @@
       <c r="E31" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>221</v>
       </c>
@@ -28583,8 +28679,11 @@
       <c r="E32" t="s">
         <v>1258</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>222</v>
       </c>
@@ -28600,8 +28699,11 @@
       <c r="E33" t="s">
         <v>1240</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -28617,8 +28719,11 @@
       <c r="E34" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -28634,8 +28739,11 @@
       <c r="E35" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>223</v>
       </c>
@@ -28651,8 +28759,11 @@
       <c r="E36" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>223</v>
       </c>
@@ -28668,8 +28779,11 @@
       <c r="E37" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>223</v>
       </c>
@@ -28685,8 +28799,11 @@
       <c r="E38" t="s">
         <v>1886</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>1651</v>
       </c>
@@ -28702,8 +28819,11 @@
       <c r="E39" t="s">
         <v>1658</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>1651</v>
       </c>
@@ -28719,8 +28839,11 @@
       <c r="E40" t="s">
         <v>1657</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>224</v>
       </c>
@@ -28736,8 +28859,11 @@
       <c r="E41" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>224</v>
       </c>
@@ -28753,8 +28879,11 @@
       <c r="E42" t="s">
         <v>990</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>224</v>
       </c>
@@ -28770,8 +28899,11 @@
       <c r="E43" t="s">
         <v>1847</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -28787,8 +28919,11 @@
       <c r="E44" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>224</v>
       </c>
@@ -28804,8 +28939,11 @@
       <c r="E45" t="s">
         <v>1642</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>224</v>
       </c>
@@ -28821,8 +28959,11 @@
       <c r="E46" t="s">
         <v>1558</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>225</v>
       </c>
@@ -28838,8 +28979,11 @@
       <c r="E47" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>225</v>
       </c>
@@ -28855,8 +28999,11 @@
       <c r="E48" t="s">
         <v>992</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>225</v>
       </c>
@@ -28872,8 +29019,11 @@
       <c r="E49" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>225</v>
       </c>
@@ -28889,8 +29039,11 @@
       <c r="E50" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>697</v>
       </c>
@@ -28906,8 +29059,11 @@
       <c r="E51" t="s">
         <v>1993</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>697</v>
       </c>
@@ -28923,8 +29079,11 @@
       <c r="E52" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>697</v>
       </c>
@@ -28940,8 +29099,11 @@
       <c r="E53" t="s">
         <v>1257</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>697</v>
       </c>
@@ -28957,8 +29119,11 @@
       <c r="E54" t="s">
         <v>1702</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>697</v>
       </c>
@@ -28974,8 +29139,11 @@
       <c r="E55" t="s">
         <v>1876</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>697</v>
       </c>
@@ -28991,8 +29159,11 @@
       <c r="E56" t="s">
         <v>1706</v>
       </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>697</v>
       </c>
@@ -29008,8 +29179,11 @@
       <c r="E57" t="s">
         <v>1709</v>
       </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>697</v>
       </c>
@@ -29025,8 +29199,11 @@
       <c r="E58" t="s">
         <v>1877</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>254</v>
       </c>
@@ -29042,8 +29219,11 @@
       <c r="E59" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>254</v>
       </c>
@@ -29059,8 +29239,11 @@
       <c r="E60" t="s">
         <v>1388</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>254</v>
       </c>
@@ -29076,8 +29259,11 @@
       <c r="E61" t="s">
         <v>1784</v>
       </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>254</v>
       </c>
@@ -29093,8 +29279,11 @@
       <c r="E62" t="s">
         <v>1713</v>
       </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>254</v>
       </c>
@@ -29110,8 +29299,11 @@
       <c r="E63" t="s">
         <v>1936</v>
       </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>255</v>
       </c>
@@ -29127,8 +29319,11 @@
       <c r="E64" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>255</v>
       </c>
@@ -29144,8 +29339,11 @@
       <c r="E65" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>255</v>
       </c>
@@ -29161,8 +29359,11 @@
       <c r="E66" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>255</v>
       </c>
@@ -29178,8 +29379,11 @@
       <c r="E67" t="s">
         <v>1864</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>255</v>
       </c>
@@ -29195,8 +29399,11 @@
       <c r="E68" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>255</v>
       </c>
@@ -29212,8 +29419,11 @@
       <c r="E69" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>255</v>
       </c>
@@ -29229,8 +29439,11 @@
       <c r="E70" t="s">
         <v>1259</v>
       </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="F70" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>255</v>
       </c>
@@ -29246,8 +29459,11 @@
       <c r="E71" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="F71" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>255</v>
       </c>
@@ -29263,8 +29479,11 @@
       <c r="E72" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="F72" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>255</v>
       </c>
@@ -29280,8 +29499,11 @@
       <c r="E73" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="F73" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>255</v>
       </c>
@@ -29297,8 +29519,11 @@
       <c r="E74" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>226</v>
       </c>
@@ -29314,8 +29539,11 @@
       <c r="E75" t="s">
         <v>1431</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="F75" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>226</v>
       </c>
@@ -29331,8 +29559,11 @@
       <c r="E76" t="s">
         <v>1139</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="F76" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>228</v>
       </c>
@@ -29348,8 +29579,11 @@
       <c r="E77" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="F77" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>228</v>
       </c>
@@ -29365,8 +29599,11 @@
       <c r="E78" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="F78" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>229</v>
       </c>
@@ -29382,8 +29619,11 @@
       <c r="E79" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="F79" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>227</v>
       </c>
@@ -29399,8 +29639,11 @@
       <c r="E80" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="F80" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>1454</v>
       </c>
@@ -29416,8 +29659,11 @@
       <c r="E81" t="s">
         <v>1635</v>
       </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="F81" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>1454</v>
       </c>
@@ -29433,8 +29679,11 @@
       <c r="E82" t="s">
         <v>1916</v>
       </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="F82" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>1940</v>
       </c>
@@ -29450,8 +29699,11 @@
       <c r="E83" t="s">
         <v>1944</v>
       </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="F83" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>230</v>
       </c>
@@ -29467,8 +29719,11 @@
       <c r="E84" t="s">
         <v>1428</v>
       </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="F84" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>230</v>
       </c>
@@ -29484,8 +29739,11 @@
       <c r="E85" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="F85" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>230</v>
       </c>
@@ -29501,8 +29759,11 @@
       <c r="E86" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="F86" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
         <v>231</v>
       </c>
@@ -29518,8 +29779,11 @@
       <c r="E87" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="F87" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>231</v>
       </c>
@@ -29535,8 +29799,11 @@
       <c r="E88" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="F88" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>231</v>
       </c>
@@ -29552,8 +29819,11 @@
       <c r="E89" t="s">
         <v>986</v>
       </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="F89" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>231</v>
       </c>
@@ -29569,8 +29839,11 @@
       <c r="E90" t="s">
         <v>1243</v>
       </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="F90" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>231</v>
       </c>
@@ -29586,8 +29859,11 @@
       <c r="E91" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="F91" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>231</v>
       </c>
@@ -29603,8 +29879,11 @@
       <c r="E92" t="s">
         <v>1246</v>
       </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="F92" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>231</v>
       </c>
@@ -29620,8 +29899,11 @@
       <c r="E93" t="s">
         <v>1248</v>
       </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="F93" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>231</v>
       </c>
@@ -29637,8 +29919,11 @@
       <c r="E94" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="F94" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>232</v>
       </c>
@@ -29654,8 +29939,11 @@
       <c r="E95" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="F95" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>232</v>
       </c>
@@ -29671,8 +29959,11 @@
       <c r="E96" t="s">
         <v>1207</v>
       </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="F96" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>232</v>
       </c>
@@ -29688,8 +29979,11 @@
       <c r="E97" t="s">
         <v>1125</v>
       </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="F97" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>233</v>
       </c>
@@ -29705,8 +29999,11 @@
       <c r="E98" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="F98" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>233</v>
       </c>
@@ -29722,8 +30019,11 @@
       <c r="E99" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="F99" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>233</v>
       </c>
@@ -29739,8 +30039,11 @@
       <c r="E100" t="s">
         <v>994</v>
       </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="F100" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>233</v>
       </c>
@@ -29756,8 +30059,11 @@
       <c r="E101" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="F101" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>233</v>
       </c>
@@ -29773,8 +30079,11 @@
       <c r="E102" t="s">
         <v>1529</v>
       </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="F102" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>233</v>
       </c>
@@ -29790,8 +30099,11 @@
       <c r="E103" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="F103" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>233</v>
       </c>
@@ -29807,8 +30119,11 @@
       <c r="E104" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="F104" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>234</v>
       </c>
@@ -29824,8 +30139,11 @@
       <c r="E105" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="F105" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>234</v>
       </c>
@@ -29841,8 +30159,11 @@
       <c r="E106" t="s">
         <v>1685</v>
       </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="F106" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>234</v>
       </c>
@@ -29858,8 +30179,11 @@
       <c r="E107" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="F107" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>234</v>
       </c>
@@ -29875,8 +30199,11 @@
       <c r="E108" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="F108" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>798</v>
       </c>
@@ -29892,8 +30219,11 @@
       <c r="E109" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="F109" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>235</v>
       </c>
@@ -29909,8 +30239,11 @@
       <c r="E110" t="s">
         <v>1003</v>
       </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="F110" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>235</v>
       </c>
@@ -29926,8 +30259,11 @@
       <c r="E111" t="s">
         <v>1994</v>
       </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="F111" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>235</v>
       </c>
@@ -29943,8 +30279,11 @@
       <c r="E112" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="F112" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>235</v>
       </c>
@@ -29960,8 +30299,11 @@
       <c r="E113" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="F113" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
       <c r="A114" t="s">
         <v>235</v>
       </c>
@@ -29977,8 +30319,11 @@
       <c r="E114" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="F114" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
       <c r="A115" t="s">
         <v>235</v>
       </c>
@@ -29994,8 +30339,11 @@
       <c r="E115" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="F115" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
       <c r="A116" t="s">
         <v>235</v>
       </c>
@@ -30011,8 +30359,11 @@
       <c r="E116" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="F116" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>235</v>
       </c>
@@ -30028,8 +30379,11 @@
       <c r="E117" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="F117" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>235</v>
       </c>
@@ -30045,8 +30399,11 @@
       <c r="E118" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="F118" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>236</v>
       </c>
@@ -30062,8 +30419,11 @@
       <c r="E119" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="F119" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>236</v>
       </c>
@@ -30079,8 +30439,11 @@
       <c r="E120" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="F120" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>236</v>
       </c>
@@ -30096,8 +30459,11 @@
       <c r="E121" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="F121" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>236</v>
       </c>
@@ -30113,8 +30479,11 @@
       <c r="E122" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="F122" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>236</v>
       </c>
@@ -30130,8 +30499,11 @@
       <c r="E123" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="F123" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>236</v>
       </c>
@@ -30147,8 +30519,11 @@
       <c r="E124" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="F124" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>236</v>
       </c>
@@ -30164,8 +30539,11 @@
       <c r="E125" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="126" spans="1:5">
+      <c r="F125" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>236</v>
       </c>
@@ -30181,8 +30559,11 @@
       <c r="E126" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="F126" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>236</v>
       </c>
@@ -30198,8 +30579,11 @@
       <c r="E127" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="F127" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
         <v>236</v>
       </c>
@@ -30215,8 +30599,11 @@
       <c r="E128" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="F128" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>238</v>
       </c>
@@ -30232,8 +30619,11 @@
       <c r="E129" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="F129" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>238</v>
       </c>
@@ -30249,8 +30639,11 @@
       <c r="E130" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="F130" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>238</v>
       </c>
@@ -30266,8 +30659,11 @@
       <c r="E131" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="F131" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>238</v>
       </c>
@@ -30283,8 +30679,11 @@
       <c r="E132" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="F132" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>238</v>
       </c>
@@ -30300,8 +30699,11 @@
       <c r="E133" t="s">
         <v>702</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="F133" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>239</v>
       </c>
@@ -30317,8 +30719,11 @@
       <c r="E134" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="F134" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>239</v>
       </c>
@@ -30334,8 +30739,11 @@
       <c r="E135" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="F135" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>240</v>
       </c>
@@ -30351,8 +30759,11 @@
       <c r="E136" t="s">
         <v>1208</v>
       </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="F136" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>240</v>
       </c>
@@ -30368,8 +30779,11 @@
       <c r="E137" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="F137" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
         <v>240</v>
       </c>
@@ -30385,8 +30799,11 @@
       <c r="E138" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="F138" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
       <c r="A139" t="s">
         <v>240</v>
       </c>
@@ -30402,8 +30819,11 @@
       <c r="E139" t="s">
         <v>1575</v>
       </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="F139" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
       <c r="A140" t="s">
         <v>240</v>
       </c>
@@ -30419,8 +30839,11 @@
       <c r="E140" t="s">
         <v>1576</v>
       </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="F140" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
       <c r="A141" t="s">
         <v>240</v>
       </c>
@@ -30436,8 +30859,11 @@
       <c r="E141" t="s">
         <v>1578</v>
       </c>
-    </row>
-    <row r="142" spans="1:5">
+      <c r="F141" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
       <c r="A142" t="s">
         <v>240</v>
       </c>
@@ -30453,8 +30879,11 @@
       <c r="E142" t="s">
         <v>1580</v>
       </c>
-    </row>
-    <row r="143" spans="1:5">
+      <c r="F142" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
       <c r="A143" t="s">
         <v>237</v>
       </c>
@@ -30470,8 +30899,11 @@
       <c r="E143" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="144" spans="1:5">
+      <c r="F143" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
       <c r="A144" t="s">
         <v>237</v>
       </c>
@@ -30487,8 +30919,11 @@
       <c r="E144" t="s">
         <v>1006</v>
       </c>
-    </row>
-    <row r="145" spans="1:5">
+      <c r="F144" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
       <c r="A145" t="s">
         <v>237</v>
       </c>
@@ -30504,8 +30939,11 @@
       <c r="E145" t="s">
         <v>985</v>
       </c>
-    </row>
-    <row r="146" spans="1:5">
+      <c r="F145" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
       <c r="A146" t="s">
         <v>237</v>
       </c>
@@ -30521,8 +30959,11 @@
       <c r="E146" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="147" spans="1:5">
+      <c r="F146" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
       <c r="A147" t="s">
         <v>237</v>
       </c>
@@ -30538,8 +30979,11 @@
       <c r="E147" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="148" spans="1:5">
+      <c r="F147" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
       <c r="A148" t="s">
         <v>237</v>
       </c>
@@ -30555,8 +30999,11 @@
       <c r="E148" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="149" spans="1:5">
+      <c r="F148" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
       <c r="A149" t="s">
         <v>237</v>
       </c>
@@ -30572,8 +31019,11 @@
       <c r="E149" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="150" spans="1:5">
+      <c r="F149" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
       <c r="A150" t="s">
         <v>237</v>
       </c>
@@ -30589,8 +31039,11 @@
       <c r="E150" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="151" spans="1:5">
+      <c r="F150" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
       <c r="A151" t="s">
         <v>237</v>
       </c>
@@ -30606,8 +31059,11 @@
       <c r="E151" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="152" spans="1:5">
+      <c r="F151" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
       <c r="A152" t="s">
         <v>237</v>
       </c>
@@ -30623,8 +31079,11 @@
       <c r="E152" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="153" spans="1:5">
+      <c r="F152" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
       <c r="A153" t="s">
         <v>237</v>
       </c>
@@ -30640,8 +31099,11 @@
       <c r="E153" t="s">
         <v>1556</v>
       </c>
-    </row>
-    <row r="154" spans="1:5">
+      <c r="F153" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
       <c r="A154" t="s">
         <v>237</v>
       </c>
@@ -30657,8 +31119,11 @@
       <c r="E154" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="155" spans="1:5">
+      <c r="F154" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
       <c r="A155" t="s">
         <v>237</v>
       </c>
@@ -30674,8 +31139,11 @@
       <c r="E155" t="s">
         <v>1495</v>
       </c>
-    </row>
-    <row r="156" spans="1:5">
+      <c r="F155" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
       <c r="A156" t="s">
         <v>237</v>
       </c>
@@ -30691,8 +31159,11 @@
       <c r="E156" t="s">
         <v>1831</v>
       </c>
-    </row>
-    <row r="157" spans="1:5">
+      <c r="F156" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
       <c r="A157" t="s">
         <v>237</v>
       </c>
@@ -30708,8 +31179,11 @@
       <c r="E157" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="158" spans="1:5">
+      <c r="F157" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
       <c r="A158" t="s">
         <v>237</v>
       </c>
@@ -30725,8 +31199,11 @@
       <c r="E158" t="s">
         <v>1883</v>
       </c>
-    </row>
-    <row r="159" spans="1:5">
+      <c r="F158" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
       <c r="A159" t="s">
         <v>237</v>
       </c>
@@ -30742,8 +31219,11 @@
       <c r="E159" t="s">
         <v>1947</v>
       </c>
-    </row>
-    <row r="160" spans="1:5">
+      <c r="F159" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
       <c r="A160" t="s">
         <v>1565</v>
       </c>
@@ -30759,8 +31239,11 @@
       <c r="E160" t="s">
         <v>1586</v>
       </c>
-    </row>
-    <row r="161" spans="1:5">
+      <c r="F160" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
       <c r="A161" t="s">
         <v>1565</v>
       </c>
@@ -30776,8 +31259,11 @@
       <c r="E161" t="s">
         <v>1588</v>
       </c>
-    </row>
-    <row r="162" spans="1:5">
+      <c r="F161" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
       <c r="A162" t="s">
         <v>1565</v>
       </c>
@@ -30793,8 +31279,11 @@
       <c r="E162" t="s">
         <v>1591</v>
       </c>
-    </row>
-    <row r="163" spans="1:5">
+      <c r="F162" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
       <c r="A163" t="s">
         <v>453</v>
       </c>
@@ -30810,8 +31299,11 @@
       <c r="E163" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="164" spans="1:5">
+      <c r="F163" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
       <c r="A164" t="s">
         <v>453</v>
       </c>
@@ -30827,8 +31319,11 @@
       <c r="E164" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="165" spans="1:5">
+      <c r="F164" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
       <c r="A165" t="s">
         <v>241</v>
       </c>
@@ -30844,8 +31339,11 @@
       <c r="E165" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="166" spans="1:5">
+      <c r="F165" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
       <c r="A166" t="s">
         <v>241</v>
       </c>
@@ -30861,8 +31359,11 @@
       <c r="E166" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="167" spans="1:5">
+      <c r="F166" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
       <c r="A167" t="s">
         <v>241</v>
       </c>
@@ -30878,8 +31379,11 @@
       <c r="E167" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="168" spans="1:5">
+      <c r="F167" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
       <c r="A168" t="s">
         <v>241</v>
       </c>
@@ -30895,8 +31399,11 @@
       <c r="E168" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="169" spans="1:5">
+      <c r="F168" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
       <c r="A169" t="s">
         <v>241</v>
       </c>
@@ -30912,8 +31419,11 @@
       <c r="E169" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="170" spans="1:5">
+      <c r="F169" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
       <c r="A170" t="s">
         <v>241</v>
       </c>
@@ -30929,8 +31439,11 @@
       <c r="E170" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="171" spans="1:5">
+      <c r="F170" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
       <c r="A171" t="s">
         <v>241</v>
       </c>
@@ -30946,8 +31459,11 @@
       <c r="E171" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="172" spans="1:5">
+      <c r="F171" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
       <c r="A172" t="s">
         <v>241</v>
       </c>
@@ -30963,8 +31479,11 @@
       <c r="E172" t="s">
         <v>1643</v>
       </c>
-    </row>
-    <row r="173" spans="1:5">
+      <c r="F172" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
       <c r="A173" t="s">
         <v>241</v>
       </c>
@@ -30980,8 +31499,11 @@
       <c r="E173" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="174" spans="1:5">
+      <c r="F173" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
       <c r="A174" t="s">
         <v>241</v>
       </c>
@@ -30997,8 +31519,11 @@
       <c r="E174" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="175" spans="1:5">
+      <c r="F174" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
       <c r="A175" t="s">
         <v>241</v>
       </c>
@@ -31014,8 +31539,11 @@
       <c r="E175" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="176" spans="1:5">
+      <c r="F175" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
       <c r="A176" t="s">
         <v>241</v>
       </c>
@@ -31031,8 +31559,11 @@
       <c r="E176" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="177" spans="1:5">
+      <c r="F176" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
       <c r="A177" t="s">
         <v>241</v>
       </c>
@@ -31048,8 +31579,11 @@
       <c r="E177" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="178" spans="1:5">
+      <c r="F177" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6">
       <c r="A178" t="s">
         <v>241</v>
       </c>
@@ -31065,8 +31599,11 @@
       <c r="E178" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="179" spans="1:5">
+      <c r="F178" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6">
       <c r="A179" t="s">
         <v>241</v>
       </c>
@@ -31082,8 +31619,11 @@
       <c r="E179" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="180" spans="1:5">
+      <c r="F179" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6">
       <c r="A180" t="s">
         <v>241</v>
       </c>
@@ -31099,8 +31639,11 @@
       <c r="E180" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="181" spans="1:5">
+      <c r="F180" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6">
       <c r="A181" t="s">
         <v>241</v>
       </c>
@@ -31116,8 +31659,11 @@
       <c r="E181" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="182" spans="1:5">
+      <c r="F181" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6">
       <c r="A182" t="s">
         <v>241</v>
       </c>
@@ -31133,8 +31679,11 @@
       <c r="E182" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="183" spans="1:5">
+      <c r="F182" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6">
       <c r="A183" t="s">
         <v>241</v>
       </c>
@@ -31150,8 +31699,11 @@
       <c r="E183" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="184" spans="1:5">
+      <c r="F183" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6">
       <c r="A184" t="s">
         <v>243</v>
       </c>
@@ -31167,8 +31719,11 @@
       <c r="E184" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="185" spans="1:5">
+      <c r="F184" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6">
       <c r="A185" t="s">
         <v>243</v>
       </c>
@@ -31184,8 +31739,11 @@
       <c r="E185" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="186" spans="1:5">
+      <c r="F185" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6">
       <c r="A186" t="s">
         <v>243</v>
       </c>
@@ -31201,8 +31759,11 @@
       <c r="E186" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="187" spans="1:5">
+      <c r="F186" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6">
       <c r="A187" t="s">
         <v>244</v>
       </c>
@@ -31218,8 +31779,11 @@
       <c r="E187" t="s">
         <v>1437</v>
       </c>
-    </row>
-    <row r="188" spans="1:5">
+      <c r="F187" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6">
       <c r="A188" t="s">
         <v>244</v>
       </c>
@@ -31235,8 +31799,11 @@
       <c r="E188" t="s">
         <v>1047</v>
       </c>
-    </row>
-    <row r="189" spans="1:5">
+      <c r="F188" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6">
       <c r="A189" t="s">
         <v>244</v>
       </c>
@@ -31252,8 +31819,11 @@
       <c r="E189" t="s">
         <v>1048</v>
       </c>
-    </row>
-    <row r="190" spans="1:5">
+      <c r="F189" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6">
       <c r="A190" t="s">
         <v>245</v>
       </c>
@@ -31269,8 +31839,11 @@
       <c r="E190" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="191" spans="1:5">
+      <c r="F190" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6">
       <c r="A191" t="s">
         <v>245</v>
       </c>
@@ -31286,8 +31859,11 @@
       <c r="E191" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="192" spans="1:5">
+      <c r="F191" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6">
       <c r="A192" t="s">
         <v>245</v>
       </c>
@@ -31303,8 +31879,11 @@
       <c r="E192" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="193" spans="1:5">
+      <c r="F192" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6">
       <c r="A193" t="s">
         <v>245</v>
       </c>
@@ -31320,8 +31899,11 @@
       <c r="E193" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="194" spans="1:5">
+      <c r="F193" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6">
       <c r="A194" t="s">
         <v>245</v>
       </c>
@@ -31337,8 +31919,11 @@
       <c r="E194" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="195" spans="1:5">
+      <c r="F194" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6">
       <c r="A195" t="s">
         <v>245</v>
       </c>
@@ -31354,8 +31939,11 @@
       <c r="E195" t="s">
         <v>1644</v>
       </c>
-    </row>
-    <row r="196" spans="1:5">
+      <c r="F195" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6">
       <c r="A196" t="s">
         <v>245</v>
       </c>
@@ -31371,8 +31959,11 @@
       <c r="E196" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="197" spans="1:5">
+      <c r="F196" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6">
       <c r="A197" t="s">
         <v>245</v>
       </c>
@@ -31388,8 +31979,11 @@
       <c r="E197" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="198" spans="1:5">
+      <c r="F197" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6">
       <c r="A198" t="s">
         <v>242</v>
       </c>
@@ -31405,8 +31999,11 @@
       <c r="E198" t="s">
         <v>1209</v>
       </c>
-    </row>
-    <row r="199" spans="1:5">
+      <c r="F198" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6">
       <c r="A199" t="s">
         <v>242</v>
       </c>
@@ -31422,8 +32019,11 @@
       <c r="E199" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="200" spans="1:5">
+      <c r="F199" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6">
       <c r="A200" t="s">
         <v>1224</v>
       </c>
@@ -31439,8 +32039,11 @@
       <c r="E200" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="201" spans="1:5">
+      <c r="F200" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6">
       <c r="A201" t="s">
         <v>1225</v>
       </c>
@@ -31456,8 +32059,11 @@
       <c r="E201" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="202" spans="1:5">
+      <c r="F201" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6">
       <c r="A202" t="s">
         <v>1225</v>
       </c>
@@ -31473,8 +32079,11 @@
       <c r="E202" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="203" spans="1:5">
+      <c r="F202" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6">
       <c r="A203" t="s">
         <v>1225</v>
       </c>
@@ -31490,8 +32099,11 @@
       <c r="E203" t="s">
         <v>1881</v>
       </c>
-    </row>
-    <row r="204" spans="1:5">
+      <c r="F203" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6">
       <c r="A204" t="s">
         <v>734</v>
       </c>
@@ -31507,8 +32119,11 @@
       <c r="E204" t="s">
         <v>772</v>
       </c>
-    </row>
-    <row r="205" spans="1:5">
+      <c r="F204" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6">
       <c r="A205" t="s">
         <v>734</v>
       </c>
@@ -31524,8 +32139,11 @@
       <c r="E205" t="s">
         <v>773</v>
       </c>
-    </row>
-    <row r="206" spans="1:5">
+      <c r="F205" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6">
       <c r="A206" t="s">
         <v>734</v>
       </c>
@@ -31541,8 +32159,11 @@
       <c r="E206" t="s">
         <v>774</v>
       </c>
-    </row>
-    <row r="207" spans="1:5">
+      <c r="F206" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6">
       <c r="A207" t="s">
         <v>246</v>
       </c>
@@ -31558,8 +32179,11 @@
       <c r="E207" t="s">
         <v>775</v>
       </c>
-    </row>
-    <row r="208" spans="1:5">
+      <c r="F207" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6">
       <c r="A208" t="s">
         <v>246</v>
       </c>
@@ -31575,8 +32199,11 @@
       <c r="E208" t="s">
         <v>776</v>
       </c>
-    </row>
-    <row r="209" spans="1:5">
+      <c r="F208" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6">
       <c r="A209" t="s">
         <v>246</v>
       </c>
@@ -31592,8 +32219,11 @@
       <c r="E209" t="s">
         <v>777</v>
       </c>
-    </row>
-    <row r="210" spans="1:5">
+      <c r="F209" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6">
       <c r="A210" t="s">
         <v>735</v>
       </c>
@@ -31609,8 +32239,11 @@
       <c r="E210" t="s">
         <v>779</v>
       </c>
-    </row>
-    <row r="211" spans="1:5">
+      <c r="F210" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6">
       <c r="A211" t="s">
         <v>735</v>
       </c>
@@ -31626,8 +32259,11 @@
       <c r="E211" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="212" spans="1:5">
+      <c r="F211" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6">
       <c r="A212" t="s">
         <v>735</v>
       </c>
@@ -31643,8 +32279,11 @@
       <c r="E212" t="s">
         <v>778</v>
       </c>
-    </row>
-    <row r="213" spans="1:5">
+      <c r="F212" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6">
       <c r="A213" t="s">
         <v>735</v>
       </c>
@@ -31660,8 +32299,11 @@
       <c r="E213" t="s">
         <v>1950</v>
       </c>
-    </row>
-    <row r="214" spans="1:5">
+      <c r="F213" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6">
       <c r="A214" t="s">
         <v>735</v>
       </c>
@@ -31677,8 +32319,11 @@
       <c r="E214" t="s">
         <v>1953</v>
       </c>
-    </row>
-    <row r="215" spans="1:5">
+      <c r="F214" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6">
       <c r="A215" t="s">
         <v>736</v>
       </c>
@@ -31694,8 +32339,11 @@
       <c r="E215" t="s">
         <v>781</v>
       </c>
-    </row>
-    <row r="216" spans="1:5">
+      <c r="F215" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6">
       <c r="A216" t="s">
         <v>736</v>
       </c>
@@ -31711,8 +32359,11 @@
       <c r="E216" t="s">
         <v>782</v>
       </c>
-    </row>
-    <row r="217" spans="1:5">
+      <c r="F216" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6">
       <c r="A217" t="s">
         <v>736</v>
       </c>
@@ -31728,8 +32379,11 @@
       <c r="E217" t="s">
         <v>783</v>
       </c>
-    </row>
-    <row r="218" spans="1:5">
+      <c r="F217" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6">
       <c r="A218" t="s">
         <v>247</v>
       </c>
@@ -31745,8 +32399,11 @@
       <c r="E218" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="219" spans="1:5">
+      <c r="F218" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6">
       <c r="A219" t="s">
         <v>247</v>
       </c>
@@ -31762,8 +32419,11 @@
       <c r="E219" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="220" spans="1:5">
+      <c r="F219" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6">
       <c r="A220" t="s">
         <v>247</v>
       </c>
@@ -31779,8 +32439,11 @@
       <c r="E220" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="221" spans="1:5">
+      <c r="F220" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6">
       <c r="A221" t="s">
         <v>247</v>
       </c>
@@ -31796,8 +32459,11 @@
       <c r="E221" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="222" spans="1:5">
+      <c r="F221" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6">
       <c r="A222" t="s">
         <v>247</v>
       </c>
@@ -31813,8 +32479,11 @@
       <c r="E222" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="223" spans="1:5">
+      <c r="F222" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6">
       <c r="A223" t="s">
         <v>247</v>
       </c>
@@ -31830,8 +32499,11 @@
       <c r="E223" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="224" spans="1:5">
+      <c r="F223" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6">
       <c r="A224" t="s">
         <v>247</v>
       </c>
@@ -31847,8 +32519,11 @@
       <c r="E224" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="225" spans="1:5">
+      <c r="F224" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6">
       <c r="A225" t="s">
         <v>247</v>
       </c>
@@ -31864,8 +32539,11 @@
       <c r="E225" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="226" spans="1:5">
+      <c r="F225" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6">
       <c r="A226" t="s">
         <v>247</v>
       </c>
@@ -31881,8 +32559,11 @@
       <c r="E226" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="227" spans="1:5">
+      <c r="F226" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6">
       <c r="A227" t="s">
         <v>247</v>
       </c>
@@ -31898,8 +32579,11 @@
       <c r="E227" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="228" spans="1:5">
+      <c r="F227" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6">
       <c r="A228" t="s">
         <v>247</v>
       </c>
@@ -31915,8 +32599,11 @@
       <c r="E228" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="229" spans="1:5">
+      <c r="F228" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6">
       <c r="A229" t="s">
         <v>247</v>
       </c>
@@ -31932,8 +32619,11 @@
       <c r="E229" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="230" spans="1:5">
+      <c r="F229" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6">
       <c r="A230" t="s">
         <v>247</v>
       </c>
@@ -31949,8 +32639,11 @@
       <c r="E230" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="231" spans="1:5">
+      <c r="F230" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6">
       <c r="A231" t="s">
         <v>247</v>
       </c>
@@ -31966,8 +32659,11 @@
       <c r="E231" t="s">
         <v>1868</v>
       </c>
-    </row>
-    <row r="232" spans="1:5">
+      <c r="F231" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6">
       <c r="A232" t="s">
         <v>247</v>
       </c>
@@ -31983,8 +32679,11 @@
       <c r="E232" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="233" spans="1:5">
+      <c r="F232" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6">
       <c r="A233" t="s">
         <v>247</v>
       </c>
@@ -32000,8 +32699,11 @@
       <c r="E233" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="234" spans="1:5">
+      <c r="F233" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6">
       <c r="A234" t="s">
         <v>247</v>
       </c>
@@ -32017,8 +32719,11 @@
       <c r="E234" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="235" spans="1:5">
+      <c r="F234" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6">
       <c r="A235" t="s">
         <v>247</v>
       </c>
@@ -32034,8 +32739,11 @@
       <c r="E235" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="236" spans="1:5">
+      <c r="F235" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6">
       <c r="A236" t="s">
         <v>247</v>
       </c>
@@ -32051,8 +32759,11 @@
       <c r="E236" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="237" spans="1:5">
+      <c r="F236" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6">
       <c r="A237" t="s">
         <v>247</v>
       </c>
@@ -32068,8 +32779,11 @@
       <c r="E237" t="s">
         <v>1866</v>
       </c>
-    </row>
-    <row r="238" spans="1:5">
+      <c r="F237" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6">
       <c r="A238" t="s">
         <v>247</v>
       </c>
@@ -32085,8 +32799,11 @@
       <c r="E238" t="s">
         <v>1018</v>
       </c>
-    </row>
-    <row r="239" spans="1:5">
+      <c r="F238" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6">
       <c r="A239" t="s">
         <v>247</v>
       </c>
@@ -32102,8 +32819,11 @@
       <c r="E239" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="240" spans="1:5">
+      <c r="F239" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6">
       <c r="A240" t="s">
         <v>247</v>
       </c>
@@ -32119,8 +32839,11 @@
       <c r="E240" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="241" spans="1:5">
+      <c r="F240" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6">
       <c r="A241" t="s">
         <v>247</v>
       </c>
@@ -32136,8 +32859,11 @@
       <c r="E241" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="242" spans="1:5">
+      <c r="F241" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6">
       <c r="A242" t="s">
         <v>248</v>
       </c>
@@ -32153,8 +32879,11 @@
       <c r="E242" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="243" spans="1:5">
+      <c r="F242" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6">
       <c r="A243" t="s">
         <v>248</v>
       </c>
@@ -32170,8 +32899,11 @@
       <c r="E243" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="244" spans="1:5">
+      <c r="F243" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6">
       <c r="A244" t="s">
         <v>248</v>
       </c>
@@ -32187,8 +32919,11 @@
       <c r="E244" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="245" spans="1:5">
+      <c r="F244" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6">
       <c r="A245" t="s">
         <v>248</v>
       </c>
@@ -32204,8 +32939,11 @@
       <c r="E245" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="246" spans="1:5">
+      <c r="F245" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6">
       <c r="A246" t="s">
         <v>249</v>
       </c>
@@ -32221,8 +32959,11 @@
       <c r="E246" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="247" spans="1:5">
+      <c r="F246" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6">
       <c r="A247" t="s">
         <v>249</v>
       </c>
@@ -32238,8 +32979,11 @@
       <c r="E247" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="248" spans="1:5">
+      <c r="F247" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6">
       <c r="A248" t="s">
         <v>249</v>
       </c>
@@ -32255,8 +32999,11 @@
       <c r="E248" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="249" spans="1:5">
+      <c r="F248" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6">
       <c r="A249" t="s">
         <v>249</v>
       </c>
@@ -32272,8 +33019,11 @@
       <c r="E249" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="250" spans="1:5">
+      <c r="F249" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -32289,8 +33039,11 @@
       <c r="E250" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="251" spans="1:5">
+      <c r="F250" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6">
       <c r="A251" t="s">
         <v>1387</v>
       </c>
@@ -32306,8 +33059,11 @@
       <c r="E251" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="252" spans="1:5">
+      <c r="F251" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6">
       <c r="A252" t="s">
         <v>1387</v>
       </c>
@@ -32323,8 +33079,11 @@
       <c r="E252" t="s">
         <v>1239</v>
       </c>
-    </row>
-    <row r="253" spans="1:5">
+      <c r="F252" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6">
       <c r="A253" t="s">
         <v>1387</v>
       </c>
@@ -32340,8 +33099,11 @@
       <c r="E253" t="s">
         <v>1442</v>
       </c>
-    </row>
-    <row r="254" spans="1:5">
+      <c r="F253" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6">
       <c r="A254" t="s">
         <v>1387</v>
       </c>
@@ -32357,8 +33119,11 @@
       <c r="E254" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="255" spans="1:5">
+      <c r="F254" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6">
       <c r="A255" t="s">
         <v>1908</v>
       </c>
@@ -32374,8 +33139,11 @@
       <c r="E255" t="s">
         <v>1918</v>
       </c>
-    </row>
-    <row r="256" spans="1:5">
+      <c r="F255" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6">
       <c r="A256" t="s">
         <v>1908</v>
       </c>
@@ -32391,8 +33159,11 @@
       <c r="E256" t="s">
         <v>1917</v>
       </c>
-    </row>
-    <row r="257" spans="1:5">
+      <c r="F256" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6">
       <c r="A257" t="s">
         <v>1908</v>
       </c>
@@ -32408,8 +33179,11 @@
       <c r="E257" t="s">
         <v>1928</v>
       </c>
-    </row>
-    <row r="258" spans="1:5">
+      <c r="F257" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6">
       <c r="A258" t="s">
         <v>1908</v>
       </c>
@@ -32425,8 +33199,11 @@
       <c r="E258" t="s">
         <v>1929</v>
       </c>
-    </row>
-    <row r="259" spans="1:5">
+      <c r="F258" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6">
       <c r="A259" t="s">
         <v>1911</v>
       </c>
@@ -32442,8 +33219,11 @@
       <c r="E259" t="s">
         <v>1686</v>
       </c>
-    </row>
-    <row r="260" spans="1:5">
+      <c r="F259" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6">
       <c r="A260" t="s">
         <v>1911</v>
       </c>
@@ -32459,8 +33239,11 @@
       <c r="E260" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="261" spans="1:5">
+      <c r="F260" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6">
       <c r="A261" t="s">
         <v>1911</v>
       </c>
@@ -32476,8 +33259,11 @@
       <c r="E261" t="s">
         <v>1557</v>
       </c>
-    </row>
-    <row r="262" spans="1:5">
+      <c r="F261" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6">
       <c r="A262" t="s">
         <v>1911</v>
       </c>
@@ -32493,8 +33279,11 @@
       <c r="E262" t="s">
         <v>1684</v>
       </c>
-    </row>
-    <row r="263" spans="1:5">
+      <c r="F262" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6">
       <c r="A263" t="s">
         <v>1911</v>
       </c>
@@ -32510,8 +33299,11 @@
       <c r="E263" t="s">
         <v>1930</v>
       </c>
-    </row>
-    <row r="264" spans="1:5">
+      <c r="F263" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6">
       <c r="A264" t="s">
         <v>250</v>
       </c>
@@ -32527,8 +33319,11 @@
       <c r="E264" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="265" spans="1:5">
+      <c r="F264" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6">
       <c r="A265" t="s">
         <v>250</v>
       </c>
@@ -32544,8 +33339,11 @@
       <c r="E265" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="266" spans="1:5">
+      <c r="F265" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6">
       <c r="A266" t="s">
         <v>250</v>
       </c>
@@ -32561,8 +33359,11 @@
       <c r="E266" t="s">
         <v>1004</v>
       </c>
-    </row>
-    <row r="267" spans="1:5">
+      <c r="F266" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6">
       <c r="A267" t="s">
         <v>250</v>
       </c>
@@ -32578,8 +33379,11 @@
       <c r="E267" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="268" spans="1:5">
+      <c r="F267" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6">
       <c r="A268" t="s">
         <v>250</v>
       </c>
@@ -32595,8 +33399,11 @@
       <c r="E268" t="s">
         <v>1939</v>
       </c>
-    </row>
-    <row r="269" spans="1:5">
+      <c r="F268" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6">
       <c r="A269" t="s">
         <v>251</v>
       </c>
@@ -32612,8 +33419,11 @@
       <c r="E269" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="270" spans="1:5">
+      <c r="F269" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6">
       <c r="A270" t="s">
         <v>252</v>
       </c>
@@ -32629,8 +33439,11 @@
       <c r="E270" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="271" spans="1:5">
+      <c r="F270" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6">
       <c r="A271" t="s">
         <v>252</v>
       </c>
@@ -32646,8 +33459,11 @@
       <c r="E271" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="272" spans="1:5">
+      <c r="F271" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6">
       <c r="A272" t="s">
         <v>252</v>
       </c>
@@ -32663,8 +33479,11 @@
       <c r="E272" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="273" spans="1:5">
+      <c r="F272" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6">
       <c r="A273" t="s">
         <v>252</v>
       </c>
@@ -32680,8 +33499,11 @@
       <c r="E273" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="274" spans="1:5">
+      <c r="F273" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6">
       <c r="A274" t="s">
         <v>253</v>
       </c>
@@ -32697,8 +33519,11 @@
       <c r="E274" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="275" spans="1:5">
+      <c r="F274" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6">
       <c r="A275" t="s">
         <v>253</v>
       </c>
@@ -32714,8 +33539,11 @@
       <c r="E275" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="276" spans="1:5">
+      <c r="F275" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6">
       <c r="A276" t="s">
         <v>253</v>
       </c>
@@ -32731,8 +33559,11 @@
       <c r="E276" t="s">
         <v>1210</v>
       </c>
-    </row>
-    <row r="277" spans="1:5">
+      <c r="F276" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6">
       <c r="A277" t="s">
         <v>253</v>
       </c>
@@ -32748,8 +33579,11 @@
       <c r="E277" t="s">
         <v>1211</v>
       </c>
-    </row>
-    <row r="278" spans="1:5">
+      <c r="F277" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6">
       <c r="A278" t="s">
         <v>253</v>
       </c>
@@ -32765,8 +33599,11 @@
       <c r="E278" t="s">
         <v>1253</v>
       </c>
-    </row>
-    <row r="279" spans="1:5">
+      <c r="F278" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6">
       <c r="A279" t="s">
         <v>253</v>
       </c>
@@ -32782,8 +33619,11 @@
       <c r="E279" t="s">
         <v>1255</v>
       </c>
-    </row>
-    <row r="280" spans="1:5">
+      <c r="F279" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6">
       <c r="A280" t="s">
         <v>459</v>
       </c>
@@ -32799,8 +33639,11 @@
       <c r="E280" t="s">
         <v>1212</v>
       </c>
-    </row>
-    <row r="281" spans="1:5">
+      <c r="F280" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6">
       <c r="A281" t="s">
         <v>459</v>
       </c>
@@ -32816,8 +33659,11 @@
       <c r="E281" t="s">
         <v>1612</v>
       </c>
-    </row>
-    <row r="282" spans="1:5">
+      <c r="F281" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6">
       <c r="A282" t="s">
         <v>459</v>
       </c>
@@ -32833,8 +33679,11 @@
       <c r="E282" t="s">
         <v>1201</v>
       </c>
-    </row>
-    <row r="283" spans="1:5">
+      <c r="F282" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6">
       <c r="A283" t="s">
         <v>459</v>
       </c>
@@ -32850,8 +33699,11 @@
       <c r="E283" t="s">
         <v>1249</v>
       </c>
-    </row>
-    <row r="284" spans="1:5">
+      <c r="F283" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6">
       <c r="A284" t="s">
         <v>459</v>
       </c>
@@ -32867,8 +33719,11 @@
       <c r="E284" t="s">
         <v>1445</v>
       </c>
-    </row>
-    <row r="285" spans="1:5">
+      <c r="F284" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6">
       <c r="A285" t="s">
         <v>459</v>
       </c>
@@ -32884,8 +33739,11 @@
       <c r="E285" t="s">
         <v>1402</v>
       </c>
-    </row>
-    <row r="286" spans="1:5">
+      <c r="F285" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6">
       <c r="A286" t="s">
         <v>459</v>
       </c>
@@ -32901,8 +33759,11 @@
       <c r="E286" t="s">
         <v>1448</v>
       </c>
-    </row>
-    <row r="287" spans="1:5">
+      <c r="F286" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6">
       <c r="A287" t="s">
         <v>459</v>
       </c>
@@ -32918,8 +33779,11 @@
       <c r="E287" t="s">
         <v>1449</v>
       </c>
-    </row>
-    <row r="288" spans="1:5">
+      <c r="F287" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6">
       <c r="A288" t="s">
         <v>459</v>
       </c>
@@ -32935,8 +33799,11 @@
       <c r="E288" t="s">
         <v>1747</v>
       </c>
-    </row>
-    <row r="289" spans="1:5">
+      <c r="F288" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6">
       <c r="A289" t="s">
         <v>459</v>
       </c>
@@ -32952,8 +33819,11 @@
       <c r="E289" t="s">
         <v>1748</v>
       </c>
-    </row>
-    <row r="290" spans="1:5">
+      <c r="F289" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6">
       <c r="A290" t="s">
         <v>460</v>
       </c>
@@ -32969,8 +33839,11 @@
       <c r="E290" t="s">
         <v>1123</v>
       </c>
-    </row>
-    <row r="291" spans="1:5">
+      <c r="F290" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6">
       <c r="A291" t="s">
         <v>460</v>
       </c>
@@ -32986,8 +33859,11 @@
       <c r="E291" t="s">
         <v>1172</v>
       </c>
-    </row>
-    <row r="292" spans="1:5">
+      <c r="F291" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6">
       <c r="A292" t="s">
         <v>460</v>
       </c>
@@ -33003,8 +33879,11 @@
       <c r="E292" t="s">
         <v>1128</v>
       </c>
-    </row>
-    <row r="293" spans="1:5">
+      <c r="F292" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6">
       <c r="A293" t="s">
         <v>1293</v>
       </c>
@@ -33020,8 +33899,11 @@
       <c r="E293" t="s">
         <v>1896</v>
       </c>
-    </row>
-    <row r="294" spans="1:5">
+      <c r="F293" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6">
       <c r="A294" t="s">
         <v>1293</v>
       </c>
@@ -33037,8 +33919,11 @@
       <c r="E294" t="s">
         <v>1897</v>
       </c>
-    </row>
-    <row r="295" spans="1:5">
+      <c r="F294" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6">
       <c r="A295" t="s">
         <v>1294</v>
       </c>
@@ -33054,8 +33939,11 @@
       <c r="E295" t="s">
         <v>1853</v>
       </c>
-    </row>
-    <row r="296" spans="1:5">
+      <c r="F295" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6">
       <c r="A296" t="s">
         <v>1294</v>
       </c>
@@ -33071,8 +33959,11 @@
       <c r="E296" t="s">
         <v>1856</v>
       </c>
-    </row>
-    <row r="297" spans="1:5">
+      <c r="F296" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6">
       <c r="A297" t="s">
         <v>1294</v>
       </c>
@@ -33088,8 +33979,11 @@
       <c r="E297" t="s">
         <v>1858</v>
       </c>
-    </row>
-    <row r="298" spans="1:5">
+      <c r="F297" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6">
       <c r="A298" t="s">
         <v>1294</v>
       </c>
@@ -33105,8 +33999,11 @@
       <c r="E298" t="s">
         <v>1859</v>
       </c>
-    </row>
-    <row r="299" spans="1:5">
+      <c r="F298" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6">
       <c r="A299" t="s">
         <v>1829</v>
       </c>
@@ -33122,9 +34019,13 @@
       <c r="E299" t="s">
         <v>1832</v>
       </c>
+      <c r="F299" t="s">
+        <v>916</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Agregar boton Ver en el Mapa
</commit_message>
<xml_diff>
--- a/Catalogo_Normalizado.xlsx
+++ b/Catalogo_Normalizado.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9388" uniqueCount="3608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9476" uniqueCount="3696">
   <si>
     <t>01</t>
   </si>
@@ -10876,6 +10876,270 @@
   </si>
   <si>
     <t>DBYF</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/288</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/187</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/277</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/250</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/30</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/280</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/198</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/254</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/299</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/351</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/86</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/149</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/278</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/77</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/18</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/123</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/122</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/376</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/13</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/147</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/148</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/256</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/252</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/22</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/210</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/10</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/242</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/261</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/76</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/165</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/263</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/264</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/276</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/262</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/36</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/128</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/127</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/15</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/map/345</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/182</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/183</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/185</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/173</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/164</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/9</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/300</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/11</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/39</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/255</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/359</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/21</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/14</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/7</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/120</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/16</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/373</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/355</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/166</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/265</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/266</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/268</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/192</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/245</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/247</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/358</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/167</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/168</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/169</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/170</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/248</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/249</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/251</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/260</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/271</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/272</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/273</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/275</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/281</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/282</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/12</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/19</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/172</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/50</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/28</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/33</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/197</t>
+  </si>
+  <si>
+    <t>https://tiles.tierradelfuego.gob.ar/catalogue/#/dataset/34</t>
   </si>
 </sst>
 </file>
@@ -28028,10 +28292,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F299"/>
+  <dimension ref="A1:G299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="F280" workbookViewId="0">
+      <selection activeCell="G295" sqref="G295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -28041,9 +28305,10 @@
     <col min="3" max="3" width="44" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>1995</v>
       </c>
@@ -28062,8 +28327,11 @@
       <c r="F1" s="1" t="s">
         <v>3607</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>3608</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>216</v>
       </c>
@@ -28083,7 +28351,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>216</v>
       </c>
@@ -28103,7 +28371,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>216</v>
       </c>
@@ -28122,8 +28390,11 @@
       <c r="F4" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>3609</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>216</v>
       </c>
@@ -28143,7 +28414,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>216</v>
       </c>
@@ -28163,7 +28434,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>216</v>
       </c>
@@ -28183,7 +28454,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -28203,7 +28474,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>217</v>
       </c>
@@ -28223,7 +28494,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>217</v>
       </c>
@@ -28243,7 +28514,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>217</v>
       </c>
@@ -28263,7 +28534,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>217</v>
       </c>
@@ -28282,8 +28553,11 @@
       <c r="F12" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" t="s">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>217</v>
       </c>
@@ -28302,8 +28576,11 @@
       <c r="F13" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="s">
+        <v>3611</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>217</v>
       </c>
@@ -28323,7 +28600,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>217</v>
       </c>
@@ -28343,7 +28620,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>218</v>
       </c>
@@ -28363,7 +28640,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>218</v>
       </c>
@@ -28383,7 +28660,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>218</v>
       </c>
@@ -28403,7 +28680,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>218</v>
       </c>
@@ -28423,7 +28700,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>218</v>
       </c>
@@ -28443,7 +28720,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>218</v>
       </c>
@@ -28463,7 +28740,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>218</v>
       </c>
@@ -28483,7 +28760,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>219</v>
       </c>
@@ -28502,8 +28779,11 @@
       <c r="F23" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" t="s">
+        <v>3612</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>219</v>
       </c>
@@ -28523,7 +28803,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>219</v>
       </c>
@@ -28543,7 +28823,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>220</v>
       </c>
@@ -28563,7 +28843,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>220</v>
       </c>
@@ -28582,8 +28862,11 @@
       <c r="F27" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" t="s">
+        <v>3613</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>220</v>
       </c>
@@ -28603,7 +28886,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>220</v>
       </c>
@@ -28623,7 +28906,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>221</v>
       </c>
@@ -28642,8 +28925,11 @@
       <c r="F30" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" t="s">
+        <v>3614</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>221</v>
       </c>
@@ -28663,7 +28949,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>221</v>
       </c>
@@ -28683,7 +28969,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>222</v>
       </c>
@@ -28703,7 +28989,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>222</v>
       </c>
@@ -28723,7 +29009,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>223</v>
       </c>
@@ -28743,7 +29029,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>223</v>
       </c>
@@ -28762,8 +29048,11 @@
       <c r="F36" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36" t="s">
+        <v>3615</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>223</v>
       </c>
@@ -28782,8 +29071,11 @@
       <c r="F37" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37" t="s">
+        <v>3616</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>223</v>
       </c>
@@ -28803,7 +29095,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>1651</v>
       </c>
@@ -28823,7 +29115,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>1651</v>
       </c>
@@ -28843,7 +29135,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>224</v>
       </c>
@@ -28863,7 +29155,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>224</v>
       </c>
@@ -28883,7 +29175,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>224</v>
       </c>
@@ -28902,8 +29194,11 @@
       <c r="F43" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43" t="s">
+        <v>3619</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>224</v>
       </c>
@@ -28922,8 +29217,11 @@
       <c r="F44" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44" t="s">
+        <v>3621</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>224</v>
       </c>
@@ -28943,7 +29241,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>224</v>
       </c>
@@ -28962,8 +29260,11 @@
       <c r="F46" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46" t="s">
+        <v>3620</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>225</v>
       </c>
@@ -28983,7 +29284,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>225</v>
       </c>
@@ -29003,7 +29304,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>225</v>
       </c>
@@ -29023,7 +29324,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>225</v>
       </c>
@@ -29043,7 +29344,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>697</v>
       </c>
@@ -29063,7 +29364,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>697</v>
       </c>
@@ -29083,7 +29384,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>697</v>
       </c>
@@ -29102,8 +29403,11 @@
       <c r="F53" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53" t="s">
+        <v>3622</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>697</v>
       </c>
@@ -29123,7 +29427,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>697</v>
       </c>
@@ -29143,7 +29447,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>697</v>
       </c>
@@ -29163,7 +29467,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>697</v>
       </c>
@@ -29183,7 +29487,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>697</v>
       </c>
@@ -29203,7 +29507,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>254</v>
       </c>
@@ -29223,7 +29527,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>254</v>
       </c>
@@ -29242,8 +29546,11 @@
       <c r="F60" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60" t="s">
+        <v>3623</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>254</v>
       </c>
@@ -29262,8 +29569,11 @@
       <c r="F61" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61" t="s">
+        <v>3624</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>254</v>
       </c>
@@ -29282,8 +29592,11 @@
       <c r="F62" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62" t="s">
+        <v>3625</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>254</v>
       </c>
@@ -29302,8 +29615,11 @@
       <c r="F63" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63" t="s">
+        <v>3626</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>255</v>
       </c>
@@ -29322,8 +29638,11 @@
       <c r="F64" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64" t="s">
+        <v>3627</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>255</v>
       </c>
@@ -29342,8 +29661,11 @@
       <c r="F65" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65" t="s">
+        <v>3629</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>255</v>
       </c>
@@ -29363,7 +29685,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>255</v>
       </c>
@@ -29382,8 +29704,11 @@
       <c r="F67" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67" t="s">
+        <v>3630</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>255</v>
       </c>
@@ -29403,7 +29728,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>255</v>
       </c>
@@ -29423,7 +29748,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>255</v>
       </c>
@@ -29443,7 +29768,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>255</v>
       </c>
@@ -29462,8 +29787,11 @@
       <c r="F71" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71" t="s">
+        <v>3628</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>255</v>
       </c>
@@ -29483,7 +29811,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>255</v>
       </c>
@@ -29503,7 +29831,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>255</v>
       </c>
@@ -29523,7 +29851,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>226</v>
       </c>
@@ -29543,7 +29871,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>226</v>
       </c>
@@ -29562,8 +29890,11 @@
       <c r="F76" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76" t="s">
+        <v>3631</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>228</v>
       </c>
@@ -29583,7 +29914,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>228</v>
       </c>
@@ -29603,7 +29934,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>229</v>
       </c>
@@ -29622,8 +29953,11 @@
       <c r="F79" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="80" spans="1:6">
+      <c r="G79" t="s">
+        <v>3633</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>227</v>
       </c>
@@ -29642,8 +29976,11 @@
       <c r="F80" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="81" spans="1:6">
+      <c r="G80" t="s">
+        <v>3632</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>1454</v>
       </c>
@@ -29663,7 +30000,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>1454</v>
       </c>
@@ -29682,8 +30019,11 @@
       <c r="F82" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="G82" t="s">
+        <v>3617</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>1940</v>
       </c>
@@ -29702,8 +30042,11 @@
       <c r="F83" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="G83" t="s">
+        <v>3618</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>230</v>
       </c>
@@ -29722,8 +30065,11 @@
       <c r="F84" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="G84" t="s">
+        <v>3639</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>230</v>
       </c>
@@ -29742,8 +30088,11 @@
       <c r="F85" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="86" spans="1:6">
+      <c r="G85" t="s">
+        <v>3640</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>230</v>
       </c>
@@ -29763,7 +30112,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>231</v>
       </c>
@@ -29782,8 +30131,11 @@
       <c r="F87" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="88" spans="1:6">
+      <c r="G87" t="s">
+        <v>3634</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>231</v>
       </c>
@@ -29802,8 +30154,11 @@
       <c r="F88" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="G88" t="s">
+        <v>3635</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>231</v>
       </c>
@@ -29823,7 +30178,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>231</v>
       </c>
@@ -29843,7 +30198,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>231</v>
       </c>
@@ -29863,7 +30218,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>231</v>
       </c>
@@ -29883,7 +30238,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>231</v>
       </c>
@@ -29903,7 +30258,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>231</v>
       </c>
@@ -29922,8 +30277,11 @@
       <c r="F94" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
+      <c r="G94" t="s">
+        <v>3636</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>232</v>
       </c>
@@ -29943,7 +30301,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>232</v>
       </c>
@@ -29963,7 +30321,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
         <v>232</v>
       </c>
@@ -29983,7 +30341,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:7">
       <c r="A98" t="s">
         <v>233</v>
       </c>
@@ -30003,7 +30361,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
         <v>233</v>
       </c>
@@ -30023,7 +30381,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:7">
       <c r="A100" t="s">
         <v>233</v>
       </c>
@@ -30042,8 +30400,11 @@
       <c r="F100" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="101" spans="1:6">
+      <c r="G100" t="s">
+        <v>3638</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
         <v>233</v>
       </c>
@@ -30063,7 +30424,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:7">
       <c r="A102" t="s">
         <v>233</v>
       </c>
@@ -30083,7 +30444,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:7">
       <c r="A103" t="s">
         <v>233</v>
       </c>
@@ -30102,8 +30463,11 @@
       <c r="F103" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="G103" t="s">
+        <v>3637</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104" t="s">
         <v>233</v>
       </c>
@@ -30123,7 +30487,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:7">
       <c r="A105" t="s">
         <v>234</v>
       </c>
@@ -30142,8 +30506,11 @@
       <c r="F105" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="106" spans="1:6">
+      <c r="G105" s="5" t="s">
+        <v>3643</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106" t="s">
         <v>234</v>
       </c>
@@ -30162,8 +30529,11 @@
       <c r="F106" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="107" spans="1:6">
+      <c r="G106" t="s">
+        <v>3642</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107" t="s">
         <v>234</v>
       </c>
@@ -30183,7 +30553,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:7">
       <c r="A108" t="s">
         <v>234</v>
       </c>
@@ -30203,7 +30573,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:7">
       <c r="A109" t="s">
         <v>798</v>
       </c>
@@ -30223,7 +30593,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:7">
       <c r="A110" t="s">
         <v>235</v>
       </c>
@@ -30242,8 +30612,11 @@
       <c r="F110" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="111" spans="1:6">
+      <c r="G110" t="s">
+        <v>3641</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111" t="s">
         <v>235</v>
       </c>
@@ -30263,7 +30636,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:7">
       <c r="A112" t="s">
         <v>235</v>
       </c>
@@ -30603,7 +30976,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="129" spans="1:6">
+    <row r="129" spans="1:7">
       <c r="A129" t="s">
         <v>238</v>
       </c>
@@ -30623,7 +30996,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="130" spans="1:6">
+    <row r="130" spans="1:7">
       <c r="A130" t="s">
         <v>238</v>
       </c>
@@ -30642,8 +31015,11 @@
       <c r="F130" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="131" spans="1:6">
+      <c r="G130" t="s">
+        <v>3648</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
       <c r="A131" t="s">
         <v>238</v>
       </c>
@@ -30663,7 +31039,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="132" spans="1:6">
+    <row r="132" spans="1:7">
       <c r="A132" t="s">
         <v>238</v>
       </c>
@@ -30682,8 +31058,11 @@
       <c r="F132" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="133" spans="1:6">
+      <c r="G132" t="s">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
       <c r="A133" t="s">
         <v>238</v>
       </c>
@@ -30702,8 +31081,11 @@
       <c r="F133" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="134" spans="1:6">
+      <c r="G133" t="s">
+        <v>3649</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
       <c r="A134" t="s">
         <v>239</v>
       </c>
@@ -30722,8 +31104,11 @@
       <c r="F134" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="135" spans="1:6">
+      <c r="G134" s="5" t="s">
+        <v>3651</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
       <c r="A135" t="s">
         <v>239</v>
       </c>
@@ -30743,7 +31128,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="136" spans="1:6">
+    <row r="136" spans="1:7">
       <c r="A136" t="s">
         <v>240</v>
       </c>
@@ -30763,7 +31148,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:7">
       <c r="A137" t="s">
         <v>240</v>
       </c>
@@ -30783,7 +31168,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:7">
       <c r="A138" t="s">
         <v>240</v>
       </c>
@@ -30803,7 +31188,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="139" spans="1:6">
+    <row r="139" spans="1:7">
       <c r="A139" t="s">
         <v>240</v>
       </c>
@@ -30823,7 +31208,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="140" spans="1:6">
+    <row r="140" spans="1:7">
       <c r="A140" t="s">
         <v>240</v>
       </c>
@@ -30843,7 +31228,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="141" spans="1:6">
+    <row r="141" spans="1:7">
       <c r="A141" t="s">
         <v>240</v>
       </c>
@@ -30863,7 +31248,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:7">
       <c r="A142" t="s">
         <v>240</v>
       </c>
@@ -30883,7 +31268,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:7">
       <c r="A143" t="s">
         <v>237</v>
       </c>
@@ -30903,7 +31288,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="144" spans="1:6">
+    <row r="144" spans="1:7">
       <c r="A144" t="s">
         <v>237</v>
       </c>
@@ -30922,8 +31307,11 @@
       <c r="F144" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="145" spans="1:6">
+      <c r="G144" t="s">
+        <v>3645</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
       <c r="A145" t="s">
         <v>237</v>
       </c>
@@ -30943,7 +31331,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:7">
       <c r="A146" t="s">
         <v>237</v>
       </c>
@@ -30963,7 +31351,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:7">
       <c r="A147" t="s">
         <v>237</v>
       </c>
@@ -30983,7 +31371,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:7">
       <c r="A148" t="s">
         <v>237</v>
       </c>
@@ -31003,7 +31391,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:7">
       <c r="A149" t="s">
         <v>237</v>
       </c>
@@ -31022,8 +31410,11 @@
       <c r="F149" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="150" spans="1:6">
+      <c r="G149" t="s">
+        <v>3644</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
       <c r="A150" t="s">
         <v>237</v>
       </c>
@@ -31043,7 +31434,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:7">
       <c r="A151" t="s">
         <v>237</v>
       </c>
@@ -31063,7 +31454,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:7">
       <c r="A152" t="s">
         <v>237</v>
       </c>
@@ -31083,7 +31474,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:7">
       <c r="A153" t="s">
         <v>237</v>
       </c>
@@ -31102,8 +31493,11 @@
       <c r="F153" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="154" spans="1:6">
+      <c r="G153" t="s">
+        <v>3646</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
       <c r="A154" t="s">
         <v>237</v>
       </c>
@@ -31123,7 +31517,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="155" spans="1:6">
+    <row r="155" spans="1:7">
       <c r="A155" t="s">
         <v>237</v>
       </c>
@@ -31143,7 +31537,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:7">
       <c r="A156" t="s">
         <v>237</v>
       </c>
@@ -31163,7 +31557,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="157" spans="1:6">
+    <row r="157" spans="1:7">
       <c r="A157" t="s">
         <v>237</v>
       </c>
@@ -31183,7 +31577,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="158" spans="1:6">
+    <row r="158" spans="1:7">
       <c r="A158" t="s">
         <v>237</v>
       </c>
@@ -31203,7 +31597,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="159" spans="1:6">
+    <row r="159" spans="1:7">
       <c r="A159" t="s">
         <v>237</v>
       </c>
@@ -31222,8 +31616,11 @@
       <c r="F159" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="160" spans="1:6">
+      <c r="G159" t="s">
+        <v>3647</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
       <c r="A160" t="s">
         <v>1565</v>
       </c>
@@ -31243,7 +31640,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:7">
       <c r="A161" t="s">
         <v>1565</v>
       </c>
@@ -31263,7 +31660,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:7">
       <c r="A162" t="s">
         <v>1565</v>
       </c>
@@ -31283,7 +31680,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="163" spans="1:6">
+    <row r="163" spans="1:7">
       <c r="A163" t="s">
         <v>453</v>
       </c>
@@ -31302,8 +31699,11 @@
       <c r="F163" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="164" spans="1:6">
+      <c r="G163" t="s">
+        <v>3655</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7">
       <c r="A164" t="s">
         <v>453</v>
       </c>
@@ -31323,7 +31723,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="165" spans="1:6">
+    <row r="165" spans="1:7">
       <c r="A165" t="s">
         <v>241</v>
       </c>
@@ -31343,7 +31743,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:7">
       <c r="A166" t="s">
         <v>241</v>
       </c>
@@ -31363,7 +31763,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:7">
       <c r="A167" t="s">
         <v>241</v>
       </c>
@@ -31382,8 +31782,11 @@
       <c r="F167" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="168" spans="1:6">
+      <c r="G167" t="s">
+        <v>3653</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7">
       <c r="A168" t="s">
         <v>241</v>
       </c>
@@ -31403,7 +31806,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="169" spans="1:6">
+    <row r="169" spans="1:7">
       <c r="A169" t="s">
         <v>241</v>
       </c>
@@ -31423,7 +31826,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="170" spans="1:6">
+    <row r="170" spans="1:7">
       <c r="A170" t="s">
         <v>241</v>
       </c>
@@ -31443,7 +31846,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="171" spans="1:6">
+    <row r="171" spans="1:7">
       <c r="A171" t="s">
         <v>241</v>
       </c>
@@ -31463,7 +31866,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:7">
       <c r="A172" t="s">
         <v>241</v>
       </c>
@@ -31483,7 +31886,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="173" spans="1:6">
+    <row r="173" spans="1:7">
       <c r="A173" t="s">
         <v>241</v>
       </c>
@@ -31503,7 +31906,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="174" spans="1:6">
+    <row r="174" spans="1:7">
       <c r="A174" t="s">
         <v>241</v>
       </c>
@@ -31523,7 +31926,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:7">
       <c r="A175" t="s">
         <v>241</v>
       </c>
@@ -31543,7 +31946,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="176" spans="1:6">
+    <row r="176" spans="1:7">
       <c r="A176" t="s">
         <v>241</v>
       </c>
@@ -31563,7 +31966,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="177" spans="1:6">
+    <row r="177" spans="1:7">
       <c r="A177" t="s">
         <v>241</v>
       </c>
@@ -31583,7 +31986,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="178" spans="1:6">
+    <row r="178" spans="1:7">
       <c r="A178" t="s">
         <v>241</v>
       </c>
@@ -31603,7 +32006,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="179" spans="1:6">
+    <row r="179" spans="1:7">
       <c r="A179" t="s">
         <v>241</v>
       </c>
@@ -31623,7 +32026,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="180" spans="1:6">
+    <row r="180" spans="1:7">
       <c r="A180" t="s">
         <v>241</v>
       </c>
@@ -31643,7 +32046,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:7">
       <c r="A181" t="s">
         <v>241</v>
       </c>
@@ -31663,7 +32066,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="182" spans="1:6">
+    <row r="182" spans="1:7">
       <c r="A182" t="s">
         <v>241</v>
       </c>
@@ -31683,7 +32086,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="183" spans="1:6">
+    <row r="183" spans="1:7">
       <c r="A183" t="s">
         <v>241</v>
       </c>
@@ -31703,7 +32106,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="184" spans="1:6">
+    <row r="184" spans="1:7">
       <c r="A184" t="s">
         <v>243</v>
       </c>
@@ -31723,7 +32126,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:7">
       <c r="A185" t="s">
         <v>243</v>
       </c>
@@ -31743,7 +32146,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:7">
       <c r="A186" t="s">
         <v>243</v>
       </c>
@@ -31763,7 +32166,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="187" spans="1:6">
+    <row r="187" spans="1:7">
       <c r="A187" t="s">
         <v>244</v>
       </c>
@@ -31783,7 +32186,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="188" spans="1:6">
+    <row r="188" spans="1:7">
       <c r="A188" t="s">
         <v>244</v>
       </c>
@@ -31803,7 +32206,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="189" spans="1:6">
+    <row r="189" spans="1:7">
       <c r="A189" t="s">
         <v>244</v>
       </c>
@@ -31823,7 +32226,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="190" spans="1:6">
+    <row r="190" spans="1:7">
       <c r="A190" t="s">
         <v>245</v>
       </c>
@@ -31842,8 +32245,11 @@
       <c r="F190" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="191" spans="1:6">
+      <c r="G190" t="s">
+        <v>3652</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7">
       <c r="A191" t="s">
         <v>245</v>
       </c>
@@ -31863,7 +32269,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="192" spans="1:6">
+    <row r="192" spans="1:7">
       <c r="A192" t="s">
         <v>245</v>
       </c>
@@ -31883,7 +32289,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="193" spans="1:6">
+    <row r="193" spans="1:7">
       <c r="A193" t="s">
         <v>245</v>
       </c>
@@ -31903,7 +32309,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:7">
       <c r="A194" t="s">
         <v>245</v>
       </c>
@@ -31923,7 +32329,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:7">
       <c r="A195" t="s">
         <v>245</v>
       </c>
@@ -31943,7 +32349,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:7">
       <c r="A196" t="s">
         <v>245</v>
       </c>
@@ -31963,7 +32369,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="197" spans="1:6">
+    <row r="197" spans="1:7">
       <c r="A197" t="s">
         <v>245</v>
       </c>
@@ -31983,7 +32389,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="198" spans="1:6">
+    <row r="198" spans="1:7">
       <c r="A198" t="s">
         <v>242</v>
       </c>
@@ -32003,7 +32409,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="199" spans="1:6">
+    <row r="199" spans="1:7">
       <c r="A199" t="s">
         <v>242</v>
       </c>
@@ -32022,8 +32428,11 @@
       <c r="F199" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="200" spans="1:6">
+      <c r="G199" t="s">
+        <v>3656</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7">
       <c r="A200" t="s">
         <v>1224</v>
       </c>
@@ -32042,8 +32451,11 @@
       <c r="F200" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="201" spans="1:6">
+      <c r="G200" t="s">
+        <v>3654</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7">
       <c r="A201" t="s">
         <v>1225</v>
       </c>
@@ -32063,7 +32475,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="202" spans="1:6">
+    <row r="202" spans="1:7">
       <c r="A202" t="s">
         <v>1225</v>
       </c>
@@ -32083,7 +32495,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="203" spans="1:6">
+    <row r="203" spans="1:7">
       <c r="A203" t="s">
         <v>1225</v>
       </c>
@@ -32103,7 +32515,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="204" spans="1:6">
+    <row r="204" spans="1:7">
       <c r="A204" t="s">
         <v>734</v>
       </c>
@@ -32123,7 +32535,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:7">
       <c r="A205" t="s">
         <v>734</v>
       </c>
@@ -32143,7 +32555,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="206" spans="1:6">
+    <row r="206" spans="1:7">
       <c r="A206" t="s">
         <v>734</v>
       </c>
@@ -32163,7 +32575,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="207" spans="1:6">
+    <row r="207" spans="1:7">
       <c r="A207" t="s">
         <v>246</v>
       </c>
@@ -32183,7 +32595,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="208" spans="1:6">
+    <row r="208" spans="1:7">
       <c r="A208" t="s">
         <v>246</v>
       </c>
@@ -32203,7 +32615,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:7">
       <c r="A209" t="s">
         <v>246</v>
       </c>
@@ -32223,7 +32635,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="210" spans="1:6">
+    <row r="210" spans="1:7">
       <c r="A210" t="s">
         <v>735</v>
       </c>
@@ -32242,8 +32654,11 @@
       <c r="F210" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="211" spans="1:6">
+      <c r="G210" t="s">
+        <v>3659</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7">
       <c r="A211" t="s">
         <v>735</v>
       </c>
@@ -32263,7 +32678,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="212" spans="1:6">
+    <row r="212" spans="1:7">
       <c r="A212" t="s">
         <v>735</v>
       </c>
@@ -32283,7 +32698,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="213" spans="1:6">
+    <row r="213" spans="1:7">
       <c r="A213" t="s">
         <v>735</v>
       </c>
@@ -32302,8 +32717,11 @@
       <c r="F213" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="214" spans="1:6">
+      <c r="G213" t="s">
+        <v>3657</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7">
       <c r="A214" t="s">
         <v>735</v>
       </c>
@@ -32322,8 +32740,11 @@
       <c r="F214" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="215" spans="1:6">
+      <c r="G214" t="s">
+        <v>3658</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7">
       <c r="A215" t="s">
         <v>736</v>
       </c>
@@ -32343,7 +32764,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="216" spans="1:6">
+    <row r="216" spans="1:7">
       <c r="A216" t="s">
         <v>736</v>
       </c>
@@ -32363,7 +32784,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="217" spans="1:6">
+    <row r="217" spans="1:7">
       <c r="A217" t="s">
         <v>736</v>
       </c>
@@ -32383,7 +32804,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="218" spans="1:6">
+    <row r="218" spans="1:7">
       <c r="A218" t="s">
         <v>247</v>
       </c>
@@ -32403,7 +32824,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="219" spans="1:6">
+    <row r="219" spans="1:7">
       <c r="A219" t="s">
         <v>247</v>
       </c>
@@ -32423,7 +32844,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="220" spans="1:6">
+    <row r="220" spans="1:7">
       <c r="A220" t="s">
         <v>247</v>
       </c>
@@ -32443,7 +32864,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="221" spans="1:6">
+    <row r="221" spans="1:7">
       <c r="A221" t="s">
         <v>247</v>
       </c>
@@ -32463,7 +32884,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="222" spans="1:6">
+    <row r="222" spans="1:7">
       <c r="A222" t="s">
         <v>247</v>
       </c>
@@ -32482,8 +32903,11 @@
       <c r="F222" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="223" spans="1:6">
+      <c r="G222" t="s">
+        <v>3674</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7">
       <c r="A223" t="s">
         <v>247</v>
       </c>
@@ -32503,7 +32927,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="224" spans="1:6">
+    <row r="224" spans="1:7">
       <c r="A224" t="s">
         <v>247</v>
       </c>
@@ -32522,8 +32946,11 @@
       <c r="F224" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="225" spans="1:6">
+      <c r="G224" t="s">
+        <v>3675</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7">
       <c r="A225" t="s">
         <v>247</v>
       </c>
@@ -32543,7 +32970,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="226" spans="1:6">
+    <row r="226" spans="1:7">
       <c r="A226" t="s">
         <v>247</v>
       </c>
@@ -32562,8 +32989,11 @@
       <c r="F226" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="227" spans="1:6">
+      <c r="G226" t="s">
+        <v>3676</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7">
       <c r="A227" t="s">
         <v>247</v>
       </c>
@@ -32583,7 +33013,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="228" spans="1:6">
+    <row r="228" spans="1:7">
       <c r="A228" t="s">
         <v>247</v>
       </c>
@@ -32602,8 +33032,11 @@
       <c r="F228" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="229" spans="1:6">
+      <c r="G228" t="s">
+        <v>3677</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7">
       <c r="A229" t="s">
         <v>247</v>
       </c>
@@ -32622,8 +33055,11 @@
       <c r="F229" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="230" spans="1:6">
+      <c r="G229" t="s">
+        <v>3686</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7">
       <c r="A230" t="s">
         <v>247</v>
       </c>
@@ -32642,8 +33078,11 @@
       <c r="F230" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="231" spans="1:6">
+      <c r="G230" t="s">
+        <v>3684</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7">
       <c r="A231" t="s">
         <v>247</v>
       </c>
@@ -32662,8 +33101,11 @@
       <c r="F231" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="232" spans="1:6">
+      <c r="G231" t="s">
+        <v>3687</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7">
       <c r="A232" t="s">
         <v>247</v>
       </c>
@@ -32682,8 +33124,11 @@
       <c r="F232" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="233" spans="1:6">
+      <c r="G232" t="s">
+        <v>3683</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7">
       <c r="A233" t="s">
         <v>247</v>
       </c>
@@ -32703,7 +33148,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="234" spans="1:6">
+    <row r="234" spans="1:7">
       <c r="A234" t="s">
         <v>247</v>
       </c>
@@ -32722,8 +33167,11 @@
       <c r="F234" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="235" spans="1:6">
+      <c r="G234" t="s">
+        <v>3679</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7">
       <c r="A235" t="s">
         <v>247</v>
       </c>
@@ -32743,7 +33191,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="236" spans="1:6">
+    <row r="236" spans="1:7">
       <c r="A236" t="s">
         <v>247</v>
       </c>
@@ -32762,8 +33210,11 @@
       <c r="F236" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="237" spans="1:6">
+      <c r="G236" t="s">
+        <v>3682</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7">
       <c r="A237" t="s">
         <v>247</v>
       </c>
@@ -32783,7 +33234,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="238" spans="1:6">
+    <row r="238" spans="1:7">
       <c r="A238" t="s">
         <v>247</v>
       </c>
@@ -32802,8 +33253,11 @@
       <c r="F238" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="239" spans="1:6">
+      <c r="G238" t="s">
+        <v>3685</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7">
       <c r="A239" t="s">
         <v>247</v>
       </c>
@@ -32822,8 +33276,11 @@
       <c r="F239" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="240" spans="1:6">
+      <c r="G239" t="s">
+        <v>3681</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7">
       <c r="A240" t="s">
         <v>247</v>
       </c>
@@ -32842,8 +33299,11 @@
       <c r="F240" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="241" spans="1:6">
+      <c r="G240" t="s">
+        <v>3678</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7">
       <c r="A241" t="s">
         <v>247</v>
       </c>
@@ -32862,8 +33322,11 @@
       <c r="F241" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="242" spans="1:6">
+      <c r="G241" t="s">
+        <v>3680</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7">
       <c r="A242" t="s">
         <v>248</v>
       </c>
@@ -32882,8 +33345,11 @@
       <c r="F242" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="243" spans="1:6">
+      <c r="G242" t="s">
+        <v>3667</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7">
       <c r="A243" t="s">
         <v>248</v>
       </c>
@@ -32903,7 +33369,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="244" spans="1:6">
+    <row r="244" spans="1:7">
       <c r="A244" t="s">
         <v>248</v>
       </c>
@@ -32922,8 +33388,11 @@
       <c r="F244" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="245" spans="1:6">
+      <c r="G244" s="5" t="s">
+        <v>3669</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7">
       <c r="A245" t="s">
         <v>248</v>
       </c>
@@ -32942,8 +33411,11 @@
       <c r="F245" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="246" spans="1:6">
+      <c r="G245" t="s">
+        <v>3668</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7">
       <c r="A246" t="s">
         <v>249</v>
       </c>
@@ -32962,8 +33434,11 @@
       <c r="F246" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="247" spans="1:6">
+      <c r="G246" t="s">
+        <v>3666</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7">
       <c r="A247" t="s">
         <v>249</v>
       </c>
@@ -32983,7 +33458,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="248" spans="1:6">
+    <row r="248" spans="1:7">
       <c r="A248" t="s">
         <v>249</v>
       </c>
@@ -33003,7 +33478,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="249" spans="1:6">
+    <row r="249" spans="1:7">
       <c r="A249" t="s">
         <v>249</v>
       </c>
@@ -33023,7 +33498,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="250" spans="1:6">
+    <row r="250" spans="1:7">
       <c r="A250" t="s">
         <v>249</v>
       </c>
@@ -33043,7 +33518,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="251" spans="1:6">
+    <row r="251" spans="1:7">
       <c r="A251" t="s">
         <v>1387</v>
       </c>
@@ -33063,7 +33538,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="252" spans="1:6">
+    <row r="252" spans="1:7">
       <c r="A252" t="s">
         <v>1387</v>
       </c>
@@ -33082,8 +33557,11 @@
       <c r="F252" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="253" spans="1:6">
+      <c r="G252" t="s">
+        <v>3661</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7">
       <c r="A253" t="s">
         <v>1387</v>
       </c>
@@ -33103,7 +33581,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="254" spans="1:6">
+    <row r="254" spans="1:7">
       <c r="A254" t="s">
         <v>1387</v>
       </c>
@@ -33122,8 +33600,11 @@
       <c r="F254" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="255" spans="1:6">
+      <c r="G254" t="s">
+        <v>3660</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7">
       <c r="A255" t="s">
         <v>1908</v>
       </c>
@@ -33142,8 +33623,11 @@
       <c r="F255" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="256" spans="1:6">
+      <c r="G255" t="s">
+        <v>3663</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7">
       <c r="A256" t="s">
         <v>1908</v>
       </c>
@@ -33162,8 +33646,11 @@
       <c r="F256" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="257" spans="1:6">
+      <c r="G256" t="s">
+        <v>3662</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7">
       <c r="A257" t="s">
         <v>1908</v>
       </c>
@@ -33182,8 +33669,11 @@
       <c r="F257" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="258" spans="1:6">
+      <c r="G257" t="s">
+        <v>3664</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7">
       <c r="A258" t="s">
         <v>1908</v>
       </c>
@@ -33202,8 +33692,11 @@
       <c r="F258" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="259" spans="1:6">
+      <c r="G258" t="s">
+        <v>3665</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7">
       <c r="A259" t="s">
         <v>1911</v>
       </c>
@@ -33222,8 +33715,11 @@
       <c r="F259" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="260" spans="1:6">
+      <c r="G259" t="s">
+        <v>3670</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7">
       <c r="A260" t="s">
         <v>1911</v>
       </c>
@@ -33243,7 +33739,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="261" spans="1:6">
+    <row r="261" spans="1:7">
       <c r="A261" t="s">
         <v>1911</v>
       </c>
@@ -33262,8 +33758,11 @@
       <c r="F261" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="262" spans="1:6">
+      <c r="G261" t="s">
+        <v>3671</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7">
       <c r="A262" t="s">
         <v>1911</v>
       </c>
@@ -33282,8 +33781,11 @@
       <c r="F262" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="263" spans="1:6">
+      <c r="G262" t="s">
+        <v>3672</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7">
       <c r="A263" t="s">
         <v>1911</v>
       </c>
@@ -33302,8 +33804,11 @@
       <c r="F263" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="264" spans="1:6">
+      <c r="G263" t="s">
+        <v>3673</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7">
       <c r="A264" t="s">
         <v>250</v>
       </c>
@@ -33322,8 +33827,11 @@
       <c r="F264" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="265" spans="1:6">
+      <c r="G264" t="s">
+        <v>3688</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7">
       <c r="A265" t="s">
         <v>250</v>
       </c>
@@ -33343,7 +33851,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="266" spans="1:6">
+    <row r="266" spans="1:7">
       <c r="A266" t="s">
         <v>250</v>
       </c>
@@ -33362,8 +33870,11 @@
       <c r="F266" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="267" spans="1:6">
+      <c r="G266" t="s">
+        <v>3689</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7">
       <c r="A267" t="s">
         <v>250</v>
       </c>
@@ -33382,8 +33893,11 @@
       <c r="F267" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="268" spans="1:6">
+      <c r="G267" t="s">
+        <v>3690</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7">
       <c r="A268" t="s">
         <v>250</v>
       </c>
@@ -33403,7 +33917,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="269" spans="1:6">
+    <row r="269" spans="1:7">
       <c r="A269" t="s">
         <v>251</v>
       </c>
@@ -33423,7 +33937,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="270" spans="1:6">
+    <row r="270" spans="1:7">
       <c r="A270" t="s">
         <v>252</v>
       </c>
@@ -33442,8 +33956,11 @@
       <c r="F270" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="271" spans="1:6">
+      <c r="G270" t="s">
+        <v>3691</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7">
       <c r="A271" t="s">
         <v>252</v>
       </c>
@@ -33463,7 +33980,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="272" spans="1:6">
+    <row r="272" spans="1:7">
       <c r="A272" t="s">
         <v>252</v>
       </c>
@@ -33483,7 +34000,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="273" spans="1:6">
+    <row r="273" spans="1:7">
       <c r="A273" t="s">
         <v>252</v>
       </c>
@@ -33503,7 +34020,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="274" spans="1:6">
+    <row r="274" spans="1:7">
       <c r="A274" t="s">
         <v>253</v>
       </c>
@@ -33523,7 +34040,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="275" spans="1:6">
+    <row r="275" spans="1:7">
       <c r="A275" t="s">
         <v>253</v>
       </c>
@@ -33543,7 +34060,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="276" spans="1:6">
+    <row r="276" spans="1:7">
       <c r="A276" t="s">
         <v>253</v>
       </c>
@@ -33563,7 +34080,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="277" spans="1:6">
+    <row r="277" spans="1:7">
       <c r="A277" t="s">
         <v>253</v>
       </c>
@@ -33583,7 +34100,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="278" spans="1:6">
+    <row r="278" spans="1:7">
       <c r="A278" t="s">
         <v>253</v>
       </c>
@@ -33603,7 +34120,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="279" spans="1:6">
+    <row r="279" spans="1:7">
       <c r="A279" t="s">
         <v>253</v>
       </c>
@@ -33623,7 +34140,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="280" spans="1:6">
+    <row r="280" spans="1:7">
       <c r="A280" t="s">
         <v>459</v>
       </c>
@@ -33643,7 +34160,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="281" spans="1:6">
+    <row r="281" spans="1:7">
       <c r="A281" t="s">
         <v>459</v>
       </c>
@@ -33663,7 +34180,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="282" spans="1:6">
+    <row r="282" spans="1:7">
       <c r="A282" t="s">
         <v>459</v>
       </c>
@@ -33682,8 +34199,11 @@
       <c r="F282" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="283" spans="1:6">
+      <c r="G282" t="s">
+        <v>3692</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7">
       <c r="A283" t="s">
         <v>459</v>
       </c>
@@ -33703,7 +34223,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="284" spans="1:6">
+    <row r="284" spans="1:7">
       <c r="A284" t="s">
         <v>459</v>
       </c>
@@ -33723,7 +34243,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="285" spans="1:6">
+    <row r="285" spans="1:7">
       <c r="A285" t="s">
         <v>459</v>
       </c>
@@ -33743,7 +34263,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="286" spans="1:6">
+    <row r="286" spans="1:7">
       <c r="A286" t="s">
         <v>459</v>
       </c>
@@ -33763,7 +34283,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="287" spans="1:6">
+    <row r="287" spans="1:7">
       <c r="A287" t="s">
         <v>459</v>
       </c>
@@ -33783,7 +34303,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="288" spans="1:6">
+    <row r="288" spans="1:7">
       <c r="A288" t="s">
         <v>459</v>
       </c>
@@ -33803,7 +34323,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="289" spans="1:6">
+    <row r="289" spans="1:7">
       <c r="A289" t="s">
         <v>459</v>
       </c>
@@ -33823,7 +34343,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="290" spans="1:6">
+    <row r="290" spans="1:7">
       <c r="A290" t="s">
         <v>460</v>
       </c>
@@ -33843,7 +34363,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="291" spans="1:6">
+    <row r="291" spans="1:7">
       <c r="A291" t="s">
         <v>460</v>
       </c>
@@ -33863,7 +34383,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="292" spans="1:6">
+    <row r="292" spans="1:7">
       <c r="A292" t="s">
         <v>460</v>
       </c>
@@ -33883,7 +34403,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="293" spans="1:6">
+    <row r="293" spans="1:7">
       <c r="A293" t="s">
         <v>1293</v>
       </c>
@@ -33902,8 +34422,11 @@
       <c r="F293" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="294" spans="1:6">
+      <c r="G293" t="s">
+        <v>3693</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7">
       <c r="A294" t="s">
         <v>1293</v>
       </c>
@@ -33922,8 +34445,11 @@
       <c r="F294" t="s">
         <v>920</v>
       </c>
-    </row>
-    <row r="295" spans="1:6">
+      <c r="G294" t="s">
+        <v>3694</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7">
       <c r="A295" t="s">
         <v>1294</v>
       </c>
@@ -33942,8 +34468,11 @@
       <c r="F295" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="296" spans="1:6">
+      <c r="G295" s="5" t="s">
+        <v>3695</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7">
       <c r="A296" t="s">
         <v>1294</v>
       </c>
@@ -33963,7 +34492,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="297" spans="1:6">
+    <row r="297" spans="1:7">
       <c r="A297" t="s">
         <v>1294</v>
       </c>
@@ -33983,7 +34512,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="298" spans="1:6">
+    <row r="298" spans="1:7">
       <c r="A298" t="s">
         <v>1294</v>
       </c>
@@ -34003,7 +34532,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="299" spans="1:6">
+    <row r="299" spans="1:7">
       <c r="A299" t="s">
         <v>1829</v>
       </c>

</xml_diff>